<commit_message>
Household masters by age group narrowing down
</commit_message>
<xml_diff>
--- a/data/processed/poland/D/households_by_master.xlsx
+++ b/data/processed/poland/D/households_by_master.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="44">
   <si>
     <t xml:space="preserve">Płeć głównego gospodarza</t>
   </si>
@@ -101,6 +101,15 @@
   </si>
   <si>
     <t xml:space="preserve">Probability within headcount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">young</t>
+  </si>
+  <si>
+    <t xml:space="preserve">middle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">elderly</t>
   </si>
   <si>
     <t xml:space="preserve">TABL. 11. GOSPODARSTWA DOMOWE WEDŁUG LICZBY OSÓB ORAZ PŁCI I WIEKU REPREZENTANTA GOSPODARSTWA W 2011 R.</t>
@@ -374,7 +383,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="9" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="13" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="8" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -530,7 +539,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="9" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="13" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -617,9 +626,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>208080</xdr:colOff>
+      <xdr:colOff>207720</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>33480</xdr:rowOff>
+      <xdr:rowOff>33120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -631,7 +640,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="110520"/>
-          <a:ext cx="1668960" cy="370440"/>
+          <a:ext cx="1668600" cy="370080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -693,9 +702,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1328760</xdr:colOff>
+      <xdr:colOff>1328400</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>33480</xdr:rowOff>
+      <xdr:rowOff>33120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -709,7 +718,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="820080" y="0"/>
-          <a:ext cx="508680" cy="480960"/>
+          <a:ext cx="508320" cy="480600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1471,10 +1480,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G211"/>
+  <dimension ref="A1:I211"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B168" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G213" activeCellId="0" sqref="G213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1503,6 +1512,15 @@
       <c r="F1" s="7" t="s">
         <v>25</v>
       </c>
+      <c r="G1" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
@@ -1525,7 +1543,15 @@
         <f aca="false">D2/E2</f>
         <v>0.0115991828431247</v>
       </c>
-      <c r="G2" s="2"/>
+      <c r="G2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
@@ -1548,7 +1574,15 @@
         <f aca="false">D3/E3</f>
         <v>0.034878751356942</v>
       </c>
-      <c r="G3" s="4"/>
+      <c r="G3" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
@@ -1571,6 +1605,15 @@
         <f aca="false">D4/E4</f>
         <v>0.0464779342000667</v>
       </c>
+      <c r="G4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
@@ -1593,6 +1636,15 @@
         <f aca="false">D5/E5</f>
         <v>0.039592789188912</v>
       </c>
+      <c r="G5" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
@@ -1615,6 +1667,15 @@
         <f aca="false">D6/E6</f>
         <v>0.0311135044576078</v>
       </c>
+      <c r="G6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
@@ -1637,6 +1698,15 @@
         <f aca="false">D7/E7</f>
         <v>0.0246856595806515</v>
       </c>
+      <c r="G7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
@@ -1659,6 +1729,15 @@
         <f aca="false">D8/E8</f>
         <v>0.0268482190937764</v>
       </c>
+      <c r="G8" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
@@ -1681,6 +1760,15 @@
         <f aca="false">D9/E9</f>
         <v>0.0364600695780017</v>
       </c>
+      <c r="G9" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
@@ -1703,6 +1791,15 @@
         <f aca="false">D10/E10</f>
         <v>0.0394261097007462</v>
       </c>
+      <c r="G10" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
@@ -1725,6 +1822,15 @@
         <f aca="false">D11/E11</f>
         <v>0.0309425511364122</v>
       </c>
+      <c r="G11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
@@ -1747,6 +1853,15 @@
         <f aca="false">D12/E12</f>
         <v>0.0143985434777034</v>
       </c>
+      <c r="G12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
@@ -1769,6 +1884,15 @@
         <f aca="false">D13/E13</f>
         <v>0.0163345898402441</v>
       </c>
+      <c r="G13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
@@ -1791,6 +1915,15 @@
         <f aca="false">D14/E14</f>
         <v>0.0150866305955159</v>
       </c>
+      <c r="G14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
@@ -1813,6 +1946,15 @@
         <f aca="false">D15/E15</f>
         <v>0.0115607183458557</v>
       </c>
+      <c r="G15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
@@ -1835,6 +1977,15 @@
         <f aca="false">D16/E16</f>
         <v>0.00688087117812481</v>
       </c>
+      <c r="G16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
@@ -1857,6 +2008,15 @@
         <f aca="false">D17/E17</f>
         <v>0.00971442247694267</v>
       </c>
+      <c r="G17" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
@@ -1879,6 +2039,15 @@
         <f aca="false">D18/E18</f>
         <v>0.0337675547691703</v>
       </c>
+      <c r="G18" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H18" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
@@ -1901,6 +2070,15 @@
         <f aca="false">D19/E19</f>
         <v>0.0406014137839663</v>
       </c>
+      <c r="G19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H19" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
@@ -1923,6 +2101,15 @@
         <f aca="false">D20/E20</f>
         <v>0.0304125958407057</v>
       </c>
+      <c r="G20" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I20" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
@@ -1945,6 +2132,15 @@
         <f aca="false">D21/E21</f>
         <v>0.0204502910480293</v>
       </c>
+      <c r="G21" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I21" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
@@ -1967,6 +2163,15 @@
         <f aca="false">D22/E22</f>
         <v>0.015159285757024</v>
       </c>
+      <c r="G22" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H22" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I22" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
@@ -1989,6 +2194,15 @@
         <f aca="false">D23/E23</f>
         <v>0.019326272961168</v>
       </c>
+      <c r="G23" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H23" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I23" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
@@ -2011,6 +2225,15 @@
         <f aca="false">D24/E24</f>
         <v>0.035545469309605</v>
       </c>
+      <c r="G24" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H24" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I24" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
@@ -2033,6 +2256,15 @@
         <f aca="false">D25/E25</f>
         <v>0.0571240522775256</v>
       </c>
+      <c r="G25" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H25" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I25" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
@@ -2055,6 +2287,15 @@
         <f aca="false">D26/E26</f>
         <v>0.0690010342675932</v>
       </c>
+      <c r="G26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I26" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
@@ -2077,6 +2318,15 @@
         <f aca="false">D27/E27</f>
         <v>0.0510381140429606</v>
       </c>
+      <c r="G27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
@@ -2099,6 +2349,15 @@
         <f aca="false">D28/E28</f>
         <v>0.0709413544631638</v>
       </c>
+      <c r="G28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I28" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
@@ -2121,6 +2380,15 @@
         <f aca="false">D29/E29</f>
         <v>0.0725611371814926</v>
       </c>
+      <c r="G29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H29" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I29" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
@@ -2143,6 +2411,15 @@
         <f aca="false">D30/E30</f>
         <v>0.0556709490473626</v>
       </c>
+      <c r="G30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I30" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
@@ -2165,6 +2442,15 @@
         <f aca="false">D31/E31</f>
         <v>0.0323999281996051</v>
       </c>
+      <c r="G31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I31" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
@@ -2187,6 +2473,15 @@
         <f aca="false">D32/E32</f>
         <v>0.00213421960468062</v>
       </c>
+      <c r="G32" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I32" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
@@ -2209,6 +2504,15 @@
         <f aca="false">D33/E33</f>
         <v>0.0118441042183421</v>
       </c>
+      <c r="G33" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I33" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
@@ -2231,6 +2535,15 @@
         <f aca="false">D34/E34</f>
         <v>0.0336913445990803</v>
       </c>
+      <c r="G34" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I34" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
@@ -2253,6 +2566,15 @@
         <f aca="false">D35/E35</f>
         <v>0.0309298925151615</v>
       </c>
+      <c r="G35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H35" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I35" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
@@ -2275,6 +2597,15 @@
         <f aca="false">D36/E36</f>
         <v>0.0205805566077312</v>
       </c>
+      <c r="G36" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H36" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I36" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
@@ -2297,6 +2628,15 @@
         <f aca="false">D37/E37</f>
         <v>0.0141371684119207</v>
       </c>
+      <c r="G37" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H37" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I37" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
@@ -2319,6 +2659,15 @@
         <f aca="false">D38/E38</f>
         <v>0.0199003759321937</v>
       </c>
+      <c r="G38" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H38" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I38" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
@@ -2341,6 +2690,15 @@
         <f aca="false">D39/E39</f>
         <v>0.0388476843309995</v>
       </c>
+      <c r="G39" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H39" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I39" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
@@ -2363,6 +2721,15 @@
         <f aca="false">D40/E40</f>
         <v>0.0582104324238462</v>
       </c>
+      <c r="G40" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H40" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I40" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
@@ -2385,6 +2752,15 @@
         <f aca="false">D41/E41</f>
         <v>0.0677492536340791</v>
       </c>
+      <c r="G41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H41" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I41" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
@@ -2407,6 +2783,15 @@
         <f aca="false">D42/E42</f>
         <v>0.0406764335724148</v>
       </c>
+      <c r="G42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H42" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I42" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
@@ -2429,6 +2814,15 @@
         <f aca="false">D43/E43</f>
         <v>0.0394912085629452</v>
       </c>
+      <c r="G43" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H43" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I43" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
@@ -2451,6 +2845,15 @@
         <f aca="false">D44/E44</f>
         <v>0.0328075170146992</v>
       </c>
+      <c r="G44" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H44" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I44" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
@@ -2473,6 +2876,15 @@
         <f aca="false">D45/E45</f>
         <v>0.0169271310630776</v>
       </c>
+      <c r="G45" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H45" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I45" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
@@ -2495,6 +2907,15 @@
         <f aca="false">D46/E46</f>
         <v>0.00790964593948429</v>
       </c>
+      <c r="G46" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H46" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I46" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
@@ -2517,6 +2938,15 @@
         <f aca="false">D47/E47</f>
         <v>0.00289993198193245</v>
       </c>
+      <c r="G47" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H47" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I47" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
@@ -2539,6 +2969,15 @@
         <f aca="false">D48/E48</f>
         <v>0.0184870663848193</v>
       </c>
+      <c r="G48" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H48" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I48" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
@@ -2561,6 +3000,15 @@
         <f aca="false">D49/E49</f>
         <v>0.0382530353571763</v>
       </c>
+      <c r="G49" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H49" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I49" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
@@ -2583,6 +3031,15 @@
         <f aca="false">D50/E50</f>
         <v>0.0374058642163871</v>
       </c>
+      <c r="G50" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H50" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I50" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
@@ -2605,6 +3062,15 @@
         <f aca="false">D51/E51</f>
         <v>0.0301601071997328</v>
       </c>
+      <c r="G51" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H51" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I51" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
@@ -2627,6 +3093,15 @@
         <f aca="false">D52/E52</f>
         <v>0.0238103965819903</v>
       </c>
+      <c r="G52" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H52" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I52" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
@@ -2649,6 +3124,15 @@
         <f aca="false">D53/E53</f>
         <v>0.0336954175372572</v>
       </c>
+      <c r="G53" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H53" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I53" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
@@ -2671,6 +3155,15 @@
         <f aca="false">D54/E54</f>
         <v>0.0614606370889896</v>
       </c>
+      <c r="G54" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H54" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I54" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
@@ -2693,6 +3186,15 @@
         <f aca="false">D55/E55</f>
         <v>0.0857597862522045</v>
       </c>
+      <c r="G55" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H55" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I55" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
@@ -2715,6 +3217,15 @@
         <f aca="false">D56/E56</f>
         <v>0.0814587635374283</v>
       </c>
+      <c r="G56" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H56" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I56" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
@@ -2737,6 +3248,15 @@
         <f aca="false">D57/E57</f>
         <v>0.0413484683715986</v>
       </c>
+      <c r="G57" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H57" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I57" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
@@ -2759,6 +3279,15 @@
         <f aca="false">D58/E58</f>
         <v>0.0449204351527148</v>
       </c>
+      <c r="G58" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H58" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I58" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
@@ -2781,6 +3310,15 @@
         <f aca="false">D59/E59</f>
         <v>0.0339968149623457</v>
       </c>
+      <c r="G59" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H59" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I59" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
@@ -2803,6 +3341,15 @@
         <f aca="false">D60/E60</f>
         <v>0.0213544148613368</v>
       </c>
+      <c r="G60" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H60" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I60" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
@@ -2825,6 +3372,15 @@
         <f aca="false">D61/E61</f>
         <v>0.00915189208343007</v>
       </c>
+      <c r="G61" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H61" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I61" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
@@ -2847,6 +3403,15 @@
         <f aca="false">D62/E62</f>
         <v>0.00234343808405131</v>
       </c>
+      <c r="G62" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H62" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I62" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
@@ -2869,6 +3434,15 @@
         <f aca="false">D63/E63</f>
         <v>0.0104673567754292</v>
       </c>
+      <c r="G63" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H63" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I63" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
@@ -2891,6 +3465,15 @@
         <f aca="false">D64/E64</f>
         <v>0.0324378120967695</v>
       </c>
+      <c r="G64" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H64" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I64" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
@@ -2913,6 +3496,15 @@
         <f aca="false">D65/E65</f>
         <v>0.053575044988225</v>
       </c>
+      <c r="G65" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H65" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I65" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
@@ -2935,6 +3527,15 @@
         <f aca="false">D66/E66</f>
         <v>0.0460934019198834</v>
       </c>
+      <c r="G66" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H66" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I66" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
@@ -2957,6 +3558,15 @@
         <f aca="false">D67/E67</f>
         <v>0.0395607066189107</v>
       </c>
+      <c r="G67" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H67" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I67" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
@@ -2979,6 +3589,15 @@
         <f aca="false">D68/E68</f>
         <v>0.0371304745317464</v>
       </c>
+      <c r="G68" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H68" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I68" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
@@ -3001,6 +3620,15 @@
         <f aca="false">D69/E69</f>
         <v>0.0572203931189714</v>
       </c>
+      <c r="G69" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H69" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I69" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
@@ -3023,6 +3651,15 @@
         <f aca="false">D70/E70</f>
         <v>0.0595464724024001</v>
       </c>
+      <c r="G70" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H70" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I70" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
@@ -3045,6 +3682,15 @@
         <f aca="false">D71/E71</f>
         <v>0.0477019841109112</v>
       </c>
+      <c r="G71" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H71" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I71" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
@@ -3067,6 +3713,15 @@
         <f aca="false">D72/E72</f>
         <v>0.019482360565434</v>
       </c>
+      <c r="G72" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H72" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I72" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
@@ -3089,6 +3744,15 @@
         <f aca="false">D73/E73</f>
         <v>0.0163172725852462</v>
       </c>
+      <c r="G73" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H73" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I73" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
@@ -3111,6 +3775,15 @@
         <f aca="false">D74/E74</f>
         <v>0.0108781817234975</v>
       </c>
+      <c r="G74" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H74" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I74" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
@@ -3133,6 +3806,15 @@
         <f aca="false">D75/E75</f>
         <v>0.0052365715211517</v>
       </c>
+      <c r="G75" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H75" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I75" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
@@ -3155,6 +3837,15 @@
         <f aca="false">D76/E76</f>
         <v>0.00248809475590633</v>
       </c>
+      <c r="G76" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H76" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I76" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
@@ -3177,6 +3868,15 @@
         <f aca="false">D77/E77</f>
         <v>0.00340232492203005</v>
       </c>
+      <c r="G77" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H77" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I77" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
@@ -3199,6 +3899,15 @@
         <f aca="false">D78/E78</f>
         <v>0.0167628151345596</v>
       </c>
+      <c r="G78" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H78" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I78" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
@@ -3221,6 +3930,15 @@
         <f aca="false">D79/E79</f>
         <v>0.0463537839292224</v>
       </c>
+      <c r="G79" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H79" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I79" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
@@ -3243,6 +3961,15 @@
         <f aca="false">D80/E80</f>
         <v>0.0686424839286438</v>
       </c>
+      <c r="G80" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H80" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I80" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
@@ -3265,6 +3992,15 @@
         <f aca="false">D81/E81</f>
         <v>0.062856217054443</v>
       </c>
+      <c r="G81" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H81" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I81" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
@@ -3287,6 +4023,15 @@
         <f aca="false">D82/E82</f>
         <v>0.0488939550869965</v>
       </c>
+      <c r="G82" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H82" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I82" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
@@ -3309,6 +4054,15 @@
         <f aca="false">D83/E83</f>
         <v>0.0567690643027838</v>
       </c>
+      <c r="G83" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H83" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I83" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
@@ -3331,6 +4085,15 @@
         <f aca="false">D84/E84</f>
         <v>0.0783807710779237</v>
       </c>
+      <c r="G84" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H84" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I84" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
@@ -3353,6 +4116,15 @@
         <f aca="false">D85/E85</f>
         <v>0.0732772836948786</v>
       </c>
+      <c r="G85" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H85" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I85" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
@@ -3375,6 +4147,15 @@
         <f aca="false">D86/E86</f>
         <v>0.0484484125376831</v>
       </c>
+      <c r="G86" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H86" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I86" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
@@ -3397,6 +4178,15 @@
         <f aca="false">D87/E87</f>
         <v>0.0183366797243422</v>
       </c>
+      <c r="G87" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H87" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I87" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
@@ -3419,6 +4209,15 @@
         <f aca="false">D88/E88</f>
         <v>0.0157270733640777</v>
       </c>
+      <c r="G88" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H88" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I88" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
@@ -3441,6 +4240,15 @@
         <f aca="false">D89/E89</f>
         <v>0.0106293722479068</v>
       </c>
+      <c r="G89" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H89" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I89" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
@@ -3463,6 +4271,15 @@
         <f aca="false">D90/E90</f>
         <v>0.00759736840582561</v>
       </c>
+      <c r="G90" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H90" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I90" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="s">
@@ -3485,6 +4302,15 @@
         <f aca="false">D91/E91</f>
         <v>0.00344282879014946</v>
       </c>
+      <c r="G91" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H91" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I91" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="s">
@@ -3507,6 +4333,15 @@
         <f aca="false">D92/E92</f>
         <v>0.00288367978770456</v>
       </c>
+      <c r="G92" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H92" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I92" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
@@ -3529,6 +4364,15 @@
         <f aca="false">D93/E93</f>
         <v>0.00816452896948253</v>
       </c>
+      <c r="G93" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H93" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I93" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="s">
@@ -3551,6 +4395,15 @@
         <f aca="false">D94/E94</f>
         <v>0.0181424148606811</v>
       </c>
+      <c r="G94" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H94" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I94" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
@@ -3573,6 +4426,15 @@
         <f aca="false">D95/E95</f>
         <v>0.049500221141088</v>
       </c>
+      <c r="G95" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H95" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I95" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
@@ -3595,6 +4457,15 @@
         <f aca="false">D96/E96</f>
         <v>0.0747456877487837</v>
       </c>
+      <c r="G96" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H96" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I96" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="s">
@@ -3617,6 +4488,15 @@
         <f aca="false">D97/E97</f>
         <v>0.0678107032286599</v>
       </c>
+      <c r="G97" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H97" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I97" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
@@ -3639,6 +4519,15 @@
         <f aca="false">D98/E98</f>
         <v>0.065891198584697</v>
       </c>
+      <c r="G98" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H98" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I98" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
@@ -3661,6 +4550,15 @@
         <f aca="false">D99/E99</f>
         <v>0.0666607695709863</v>
       </c>
+      <c r="G99" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H99" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I99" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
@@ -3683,6 +4581,15 @@
         <f aca="false">D100/E100</f>
         <v>0.0505528527200354</v>
       </c>
+      <c r="G100" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H100" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I100" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="s">
@@ -3705,6 +4612,15 @@
         <f aca="false">D101/E101</f>
         <v>0.0297390535161433</v>
       </c>
+      <c r="G101" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H101" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I101" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="s">
@@ -3727,6 +4643,15 @@
         <f aca="false">D102/E102</f>
         <v>0.0105882352941176</v>
       </c>
+      <c r="G102" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H102" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I102" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="s">
@@ -3749,6 +4674,15 @@
         <f aca="false">D103/E103</f>
         <v>0.00597080937638213</v>
       </c>
+      <c r="G103" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H103" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I103" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="s">
@@ -3771,6 +4705,15 @@
         <f aca="false">D104/E104</f>
         <v>0.004281291463954</v>
       </c>
+      <c r="G104" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H104" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I104" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="s">
@@ -3793,6 +4736,15 @@
         <f aca="false">D105/E105</f>
         <v>0.00174259177355153</v>
       </c>
+      <c r="G105" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H105" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I105" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="s">
@@ -3815,6 +4767,15 @@
         <f aca="false">D106/E106</f>
         <v>0.000698805838124724</v>
       </c>
+      <c r="G106" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H106" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I106" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="s">
@@ -3837,6 +4798,15 @@
         <f aca="false">D107/E107</f>
         <v>0.00446704997788589</v>
       </c>
+      <c r="G107" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H107" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I107" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="s">
@@ -3859,6 +4829,15 @@
         <f aca="false">D108/E108</f>
         <v>0.0122954444935869</v>
       </c>
+      <c r="G108" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H108" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I108" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
@@ -3881,6 +4860,15 @@
         <f aca="false">D109/E109</f>
         <v>0.0332950022114109</v>
       </c>
+      <c r="G109" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H109" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I109" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
@@ -3903,6 +4891,15 @@
         <f aca="false">D110/E110</f>
         <v>0.0771605484298983</v>
       </c>
+      <c r="G110" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H110" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I110" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
@@ -3925,6 +4922,15 @@
         <f aca="false">D111/E111</f>
         <v>0.0951968155683326</v>
       </c>
+      <c r="G111" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H111" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I111" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="s">
@@ -3947,6 +4953,15 @@
         <f aca="false">D112/E112</f>
         <v>0.0722069880583812</v>
       </c>
+      <c r="G112" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H112" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I112" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="s">
@@ -3969,6 +4984,15 @@
         <f aca="false">D113/E113</f>
         <v>0.0645731977001327</v>
       </c>
+      <c r="G113" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H113" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I113" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="s">
@@ -3991,6 +5015,15 @@
         <f aca="false">D114/E114</f>
         <v>0.0689252543122512</v>
       </c>
+      <c r="G114" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H114" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I114" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="s">
@@ -4013,6 +5046,15 @@
         <f aca="false">D115/E115</f>
         <v>0.0528261831048209</v>
       </c>
+      <c r="G115" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H115" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I115" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="s">
@@ -4035,6 +5077,15 @@
         <f aca="false">D116/E116</f>
         <v>0.0302697921273773</v>
       </c>
+      <c r="G116" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H116" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I116" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="s">
@@ -4057,6 +5108,15 @@
         <f aca="false">D117/E117</f>
         <v>0.00947368421052632</v>
       </c>
+      <c r="G117" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H117" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I117" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="s">
@@ -4079,6 +5139,15 @@
         <f aca="false">D118/E118</f>
         <v>0.0101105705440071</v>
       </c>
+      <c r="G118" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H118" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I118" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
@@ -4101,6 +5170,15 @@
         <f aca="false">D119/E119</f>
         <v>0.00608580274214949</v>
       </c>
+      <c r="G119" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H119" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I119" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
@@ -4123,6 +5201,15 @@
         <f aca="false">D120/E120</f>
         <v>0.00366209641751437</v>
       </c>
+      <c r="G120" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H120" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I120" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="s">
@@ -4145,6 +5232,15 @@
         <f aca="false">D121/E121</f>
         <v>0.00207872622733304</v>
       </c>
+      <c r="G121" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H121" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I121" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="s">
@@ -4167,6 +5263,15 @@
         <f aca="false">D122/E122</f>
         <v>0.00281920219212731</v>
       </c>
+      <c r="G122" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H122" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I122" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="s">
@@ -4189,6 +5294,15 @@
         <f aca="false">D123/E123</f>
         <v>0.012278020761975</v>
       </c>
+      <c r="G123" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H123" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I123" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="s">
@@ -4211,6 +5325,15 @@
         <f aca="false">D124/E124</f>
         <v>0.0128049744427465</v>
       </c>
+      <c r="G124" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H124" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I124" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="s">
@@ -4233,6 +5356,15 @@
         <f aca="false">D125/E125</f>
         <v>0.0273225483480002</v>
       </c>
+      <c r="G125" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H125" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I125" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="s">
@@ -4255,6 +5387,15 @@
         <f aca="false">D126/E126</f>
         <v>0.0511408547188702</v>
       </c>
+      <c r="G126" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H126" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I126" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="s">
@@ -4277,6 +5418,15 @@
         <f aca="false">D127/E127</f>
         <v>0.0555672656373505</v>
       </c>
+      <c r="G127" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H127" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I127" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="s">
@@ -4299,6 +5449,15 @@
         <f aca="false">D128/E128</f>
         <v>0.0734046477314644</v>
       </c>
+      <c r="G128" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H128" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I128" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
@@ -4321,6 +5480,15 @@
         <f aca="false">D129/E129</f>
         <v>0.0700848395426042</v>
       </c>
+      <c r="G129" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H129" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I129" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="s">
@@ -4343,6 +5511,15 @@
         <f aca="false">D130/E130</f>
         <v>0.0537492754386889</v>
       </c>
+      <c r="G130" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H130" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I130" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
@@ -4365,6 +5542,15 @@
         <f aca="false">D131/E131</f>
         <v>0.0354903303999578</v>
       </c>
+      <c r="G131" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H131" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I131" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
@@ -4387,6 +5573,15 @@
         <f aca="false">D132/E132</f>
         <v>0.0154133951625652</v>
       </c>
+      <c r="G132" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H132" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I132" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="s">
@@ -4409,6 +5604,15 @@
         <f aca="false">D133/E133</f>
         <v>0.0107498550877378</v>
       </c>
+      <c r="G133" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H133" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I133" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="s">
@@ -4431,6 +5635,15 @@
         <f aca="false">D134/E134</f>
         <v>0.0063497918532961</v>
       </c>
+      <c r="G134" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H134" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I134" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
@@ -4453,6 +5666,15 @@
         <f aca="false">D135/E135</f>
         <v>0.00310902671655162</v>
       </c>
+      <c r="G135" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H135" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I135" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="s">
@@ -4475,6 +5697,15 @@
         <f aca="false">D136/E136</f>
         <v>0.00108025504558149</v>
       </c>
+      <c r="G136" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H136" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I136" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="s">
@@ -4497,6 +5728,15 @@
         <f aca="false">D137/E137</f>
         <v>0.00437371555040312</v>
       </c>
+      <c r="G137" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H137" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I137" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="s">
@@ -4519,6 +5759,15 @@
         <f aca="false">D138/E138</f>
         <v>0.0153080044264109</v>
       </c>
+      <c r="G138" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H138" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I138" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="s">
@@ -4541,6 +5790,15 @@
         <f aca="false">D139/E139</f>
         <v>0.0354376350318807</v>
       </c>
+      <c r="G139" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H139" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I139" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
@@ -4563,6 +5821,15 @@
         <f aca="false">D140/E140</f>
         <v>0.0568056067871634</v>
       </c>
+      <c r="G140" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H140" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I140" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
@@ -4585,6 +5852,15 @@
         <f aca="false">D141/E141</f>
         <v>0.0814143436791906</v>
       </c>
+      <c r="G141" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H141" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I141" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
@@ -4607,6 +5883,15 @@
         <f aca="false">D142/E142</f>
         <v>0.0660536438847025</v>
       </c>
+      <c r="G142" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H142" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I142" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
@@ -4629,6 +5914,15 @@
         <f aca="false">D143/E143</f>
         <v>0.0760394161353217</v>
       </c>
+      <c r="G143" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H143" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I143" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
@@ -4651,6 +5945,15 @@
         <f aca="false">D144/E144</f>
         <v>0.0755651578226274</v>
       </c>
+      <c r="G144" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H144" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I144" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="s">
@@ -4673,6 +5976,15 @@
         <f aca="false">D145/E145</f>
         <v>0.0671602466143226</v>
       </c>
+      <c r="G145" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H145" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I145" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
@@ -4695,6 +6007,15 @@
         <f aca="false">D146/E146</f>
         <v>0.0480845233703957</v>
       </c>
+      <c r="G146" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H146" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I146" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
@@ -4717,6 +6038,15 @@
         <f aca="false">D147/E147</f>
         <v>0.0155978289508352</v>
       </c>
+      <c r="G147" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H147" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I147" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
@@ -4739,6 +6069,15 @@
         <f aca="false">D148/E148</f>
         <v>0.0109079411919692</v>
       </c>
+      <c r="G148" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H148" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I148" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
@@ -4761,6 +6100,15 @@
         <f aca="false">D149/E149</f>
         <v>0.0100121199346577</v>
       </c>
+      <c r="G149" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H149" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I149" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
@@ -4783,6 +6131,15 @@
         <f aca="false">D150/E150</f>
         <v>0.00395215260578595</v>
       </c>
+      <c r="G150" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H150" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I150" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="s">
@@ -4805,6 +6162,15 @@
         <f aca="false">D151/E151</f>
         <v>0.00192338093481583</v>
       </c>
+      <c r="G151" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H151" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I151" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="s">
@@ -4827,6 +6193,15 @@
         <f aca="false">D152/E152</f>
         <v>0.00286468149264983</v>
       </c>
+      <c r="G152" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H152" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I152" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="s">
@@ -4849,6 +6224,15 @@
         <f aca="false">D153/E153</f>
         <v>0.0027892951375801</v>
       </c>
+      <c r="G153" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H153" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I153" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="s">
@@ -4871,6 +6255,15 @@
         <f aca="false">D154/E154</f>
         <v>0.0119864304560875</v>
       </c>
+      <c r="G154" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H154" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I154" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="s">
@@ -4893,6 +6286,15 @@
         <f aca="false">D155/E155</f>
         <v>0.0260082924990577</v>
       </c>
+      <c r="G155" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H155" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I155" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="s">
@@ -4915,6 +6317,15 @@
         <f aca="false">D156/E156</f>
         <v>0.0326422917451941</v>
       </c>
+      <c r="G156" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H156" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I156" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="s">
@@ -4937,6 +6348,15 @@
         <f aca="false">D157/E157</f>
         <v>0.0519411986430456</v>
       </c>
+      <c r="G157" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H157" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I157" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="s">
@@ -4959,6 +6379,15 @@
         <f aca="false">D158/E158</f>
         <v>0.0516396532227667</v>
       </c>
+      <c r="G158" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H158" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I158" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="s">
@@ -4981,6 +6410,15 @@
         <f aca="false">D159/E159</f>
         <v>0.0823218997361478</v>
       </c>
+      <c r="G159" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H159" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I159" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="s">
@@ -5003,6 +6441,15 @@
         <f aca="false">D160/E160</f>
         <v>0.0603844704108556</v>
       </c>
+      <c r="G160" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H160" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I160" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="s">
@@ -5025,6 +6472,15 @@
         <f aca="false">D161/E161</f>
         <v>0.0456841311722578</v>
       </c>
+      <c r="G161" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H161" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I161" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="s">
@@ -5047,6 +6503,15 @@
         <f aca="false">D162/E162</f>
         <v>0.0183942706370147</v>
       </c>
+      <c r="G162" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H162" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I162" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="s">
@@ -5069,6 +6534,15 @@
         <f aca="false">D163/E163</f>
         <v>0.0141726347531097</v>
       </c>
+      <c r="G163" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H163" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I163" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="s">
@@ -5091,6 +6565,15 @@
         <f aca="false">D164/E164</f>
         <v>0.0114587259705993</v>
       </c>
+      <c r="G164" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H164" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I164" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="s">
@@ -5113,6 +6596,15 @@
         <f aca="false">D165/E165</f>
         <v>0.00173388616660384</v>
       </c>
+      <c r="G165" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H165" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I165" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="s">
@@ -5135,6 +6627,15 @@
         <f aca="false">D166/E166</f>
         <v>0.00173388616660384</v>
       </c>
+      <c r="G166" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H166" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I166" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="s">
@@ -5157,6 +6658,15 @@
         <f aca="false">D167/E167</f>
         <v>0.00497549943460234</v>
       </c>
+      <c r="G167" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H167" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I167" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="s">
@@ -5179,6 +6689,15 @@
         <f aca="false">D168/E168</f>
         <v>0.0131926121372032</v>
       </c>
+      <c r="G168" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H168" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I168" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="s">
@@ -5201,6 +6720,15 @@
         <f aca="false">D169/E169</f>
         <v>0.0277421786656615</v>
       </c>
+      <c r="G169" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H169" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I169" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="s">
@@ -5223,6 +6751,15 @@
         <f aca="false">D170/E170</f>
         <v>0.0524689031285337</v>
       </c>
+      <c r="G170" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H170" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I170" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="s">
@@ -5245,6 +6782,15 @@
         <f aca="false">D171/E171</f>
         <v>0.071541650961176</v>
       </c>
+      <c r="G171" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H171" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I171" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="s">
@@ -5267,6 +6813,15 @@
         <f aca="false">D172/E172</f>
         <v>0.0670184696569921</v>
       </c>
+      <c r="G172" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H172" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I172" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="s">
@@ -5289,6 +6844,15 @@
         <f aca="false">D173/E173</f>
         <v>0.0813418771202412</v>
       </c>
+      <c r="G173" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H173" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I173" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="s">
@@ -5311,6 +6875,15 @@
         <f aca="false">D174/E174</f>
         <v>0.0766679231059178</v>
       </c>
+      <c r="G174" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H174" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I174" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="s">
@@ -5333,6 +6906,15 @@
         <f aca="false">D175/E175</f>
         <v>0.0811911044101018</v>
       </c>
+      <c r="G175" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H175" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I175" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="s">
@@ -5355,6 +6937,15 @@
         <f aca="false">D176/E176</f>
         <v>0.0538258575197889</v>
       </c>
+      <c r="G176" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H176" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I176" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="s">
@@ -5377,6 +6968,15 @@
         <f aca="false">D177/E177</f>
         <v>0.0219374293252921</v>
       </c>
+      <c r="G177" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H177" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I177" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="s">
@@ -5399,6 +6999,15 @@
         <f aca="false">D178/E178</f>
         <v>0.0147757255936675</v>
       </c>
+      <c r="G178" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H178" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I178" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
@@ -5421,6 +7030,15 @@
         <f aca="false">D179/E179</f>
         <v>0.0115341123256691</v>
       </c>
+      <c r="G179" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H179" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I179" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
@@ -5443,6 +7061,15 @@
         <f aca="false">D180/E180</f>
         <v>0.00505088578967207</v>
       </c>
+      <c r="G180" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H180" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I180" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="s">
@@ -5465,6 +7092,15 @@
         <f aca="false">D181/E181</f>
         <v>0.000980022615906521</v>
       </c>
+      <c r="G181" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H181" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I181" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="s">
@@ -5487,6 +7123,15 @@
         <f aca="false">D182/E182</f>
         <v>0.00420333639826612</v>
       </c>
+      <c r="G182" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H182" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I182" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="s">
@@ -5509,6 +7154,15 @@
         <f aca="false">D183/E183</f>
         <v>0.00446604492315776</v>
       </c>
+      <c r="G183" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H183" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I183" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="s">
@@ -5531,6 +7185,15 @@
         <f aca="false">D184/E184</f>
         <v>0.0118218836201235</v>
       </c>
+      <c r="G184" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H184" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I184" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
@@ -5553,6 +7216,15 @@
         <f aca="false">D185/E185</f>
         <v>0.0219361618284513</v>
       </c>
+      <c r="G185" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H185" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I185" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">
@@ -5575,6 +7247,15 @@
         <f aca="false">D186/E186</f>
         <v>0.0295547090503087</v>
       </c>
+      <c r="G186" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H186" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I186" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="s">
@@ -5597,6 +7278,15 @@
         <f aca="false">D187/E187</f>
         <v>0.0378300275843951</v>
       </c>
+      <c r="G187" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H187" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I187" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="s">
@@ -5619,6 +7309,15 @@
         <f aca="false">D188/E188</f>
         <v>0.037173256272166</v>
       </c>
+      <c r="G188" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H188" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I188" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="s">
@@ -5641,6 +7340,15 @@
         <f aca="false">D189/E189</f>
         <v>0.0697491133587285</v>
       </c>
+      <c r="G189" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H189" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I189" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="0" t="s">
@@ -5663,6 +7371,15 @@
         <f aca="false">D190/E190</f>
         <v>0.0605543149875213</v>
       </c>
+      <c r="G190" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H190" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I190" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="0" t="s">
@@ -5685,6 +7402,15 @@
         <f aca="false">D191/E191</f>
         <v>0.062918691711546</v>
       </c>
+      <c r="G191" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H191" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I191" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="0" t="s">
@@ -5707,6 +7433,15 @@
         <f aca="false">D192/E192</f>
         <v>0.0191777223170892</v>
       </c>
+      <c r="G192" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H192" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I192" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="0" t="s">
@@ -5729,6 +7464,15 @@
         <f aca="false">D193/E193</f>
         <v>0.0149743859188231</v>
       </c>
+      <c r="G193" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H193" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I193" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="0" t="s">
@@ -5751,6 +7495,15 @@
         <f aca="false">D194/E194</f>
         <v>0.0110337580454486</v>
       </c>
+      <c r="G194" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H194" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I194" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="0" t="s">
@@ -5773,6 +7526,15 @@
         <f aca="false">D195/E195</f>
         <v>0.00354656508603704</v>
       </c>
+      <c r="G195" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H195" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I195" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="0" t="s">
@@ -5795,6 +7557,15 @@
         <f aca="false">D196/E196</f>
         <v>0.00341521082359123</v>
       </c>
+      <c r="G196" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H196" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I196" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="0" t="s">
@@ -5817,6 +7588,15 @@
         <f aca="false">D197/E197</f>
         <v>0.0056482332851701</v>
       </c>
+      <c r="G197" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H197" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I197" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="0" t="s">
@@ -5839,6 +7619,15 @@
         <f aca="false">D198/E198</f>
         <v>0.0123473006699067</v>
       </c>
+      <c r="G198" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H198" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I198" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="0" t="s">
@@ -5861,6 +7650,15 @@
         <f aca="false">D199/E199</f>
         <v>0.0357283593852621</v>
       </c>
+      <c r="G199" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H199" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I199" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="s">
@@ -5883,6 +7681,15 @@
         <f aca="false">D200/E200</f>
         <v>0.0601602522001839</v>
       </c>
+      <c r="G200" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H200" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I200" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="0" t="s">
@@ -5905,6 +7712,15 @@
         <f aca="false">D201/E201</f>
         <v>0.0559569158019178</v>
       </c>
+      <c r="G201" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H201" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I201" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="0" t="s">
@@ -5927,6 +7743,15 @@
         <f aca="false">D202/E202</f>
         <v>0.0721134900827532</v>
       </c>
+      <c r="G202" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H202" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I202" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="s">
@@ -5949,6 +7774,15 @@
         <f aca="false">D203/E203</f>
         <v>0.0650203599106791</v>
       </c>
+      <c r="G203" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H203" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I203" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="s">
@@ -5971,6 +7805,15 @@
         <f aca="false">D204/E204</f>
         <v>0.0785498489425982</v>
       </c>
+      <c r="G204" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H204" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I204" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="s">
@@ -5993,6 +7836,15 @@
         <f aca="false">D205/E205</f>
         <v>0.105083409956653</v>
       </c>
+      <c r="G205" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H205" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I205" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="s">
@@ -6015,6 +7867,15 @@
         <f aca="false">D206/E206</f>
         <v>0.0609483777748588</v>
       </c>
+      <c r="G206" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H206" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I206" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="0" t="s">
@@ -6037,6 +7898,15 @@
         <f aca="false">D207/E207</f>
         <v>0.0197031393668725</v>
       </c>
+      <c r="G207" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H207" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I207" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="0" t="s">
@@ -6059,6 +7929,15 @@
         <f aca="false">D208/E208</f>
         <v>0.00893208984631551</v>
       </c>
+      <c r="G208" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H208" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I208" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="0" t="s">
@@ -6081,6 +7960,15 @@
         <f aca="false">D209/E209</f>
         <v>0.00958886115854459</v>
       </c>
+      <c r="G209" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H209" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I209" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="0" t="s">
@@ -6103,6 +7991,15 @@
         <f aca="false">D210/E210</f>
         <v>0.00945750689609878</v>
       </c>
+      <c r="G210" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H210" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I210" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="0" t="s">
@@ -6124,6 +8021,15 @@
       <c r="F211" s="0" t="n">
         <f aca="false">D211/E211</f>
         <v>0.00840667279653225</v>
+      </c>
+      <c r="G211" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H211" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I211" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -6159,7 +8065,7 @@
     <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -6189,13 +8095,13 @@
     </row>
     <row r="4" customFormat="false" ht="35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D4" s="14"/>
       <c r="E4" s="14"/>
@@ -6204,10 +8110,10 @@
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
       <c r="J4" s="6" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="K4" s="15" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="L4" s="16"/>
     </row>
@@ -6233,7 +8139,7 @@
         <v>6</v>
       </c>
       <c r="I5" s="17" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="J5" s="6"/>
       <c r="K5" s="15"/>
@@ -6241,10 +8147,10 @@
     </row>
     <row r="6" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="18" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C6" s="19"/>
       <c r="D6" s="19"/>
@@ -6259,7 +8165,7 @@
     </row>
     <row r="7" s="25" customFormat="true" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B7" s="21" t="n">
         <v>1099505</v>
@@ -6295,7 +8201,7 @@
     </row>
     <row r="8" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="26" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B8" s="27"/>
       <c r="C8" s="28"/>
@@ -6851,7 +8757,7 @@
     </row>
     <row r="24" s="25" customFormat="true" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B24" s="21" t="n">
         <v>480542</v>
@@ -6887,7 +8793,7 @@
     </row>
     <row r="25" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="26" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B25" s="27"/>
       <c r="C25" s="28"/>
@@ -7443,7 +9349,7 @@
     </row>
     <row r="41" s="25" customFormat="true" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B41" s="21" t="n">
         <v>618964</v>
@@ -7479,7 +9385,7 @@
     </row>
     <row r="42" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="26" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B42" s="27"/>
       <c r="C42" s="28"/>
@@ -8035,10 +9941,10 @@
     </row>
     <row r="58" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="18" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B58" s="31" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C58" s="31"/>
       <c r="D58" s="31"/>
@@ -8053,7 +9959,7 @@
     </row>
     <row r="59" s="25" customFormat="true" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B59" s="21" t="n">
         <v>824211</v>
@@ -8089,7 +9995,7 @@
     </row>
     <row r="60" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="26" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B60" s="27"/>
       <c r="C60" s="28"/>
@@ -8645,7 +10551,7 @@
     </row>
     <row r="76" s="25" customFormat="true" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B76" s="21" t="n">
         <v>350099</v>
@@ -8681,7 +10587,7 @@
     </row>
     <row r="77" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="26" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B77" s="27"/>
       <c r="C77" s="28"/>
@@ -9237,7 +11143,7 @@
     </row>
     <row r="93" s="25" customFormat="true" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B93" s="21" t="n">
         <v>474112</v>
@@ -9273,7 +11179,7 @@
     </row>
     <row r="94" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="26" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B94" s="27"/>
       <c r="C94" s="28"/>
@@ -9829,10 +11735,10 @@
     </row>
     <row r="110" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A110" s="18" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B110" s="31" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C110" s="31"/>
       <c r="D110" s="31"/>
@@ -9847,7 +11753,7 @@
     </row>
     <row r="111" s="25" customFormat="true" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A111" s="34" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B111" s="35" t="n">
         <v>275295</v>
@@ -9883,7 +11789,7 @@
     </row>
     <row r="112" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A112" s="38" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B112" s="39"/>
       <c r="C112" s="40"/>
@@ -10439,7 +12345,7 @@
     </row>
     <row r="128" s="25" customFormat="true" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A128" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B128" s="21" t="n">
         <v>130443</v>
@@ -10475,7 +12381,7 @@
     </row>
     <row r="129" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A129" s="26" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B129" s="27"/>
       <c r="C129" s="28"/>
@@ -11031,7 +12937,7 @@
     </row>
     <row r="145" s="25" customFormat="true" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A145" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B145" s="21" t="n">
         <v>144851</v>
@@ -11067,7 +12973,7 @@
     </row>
     <row r="146" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A146" s="26" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B146" s="27"/>
       <c r="C146" s="28"/>

</xml_diff>